<commit_message>
make some bug but i will repair them
</commit_message>
<xml_diff>
--- a/Assets/_Excel/option.xlsx
+++ b/Assets/_Excel/option.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\unity\BattleFlagGameStudy\Assets\_Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{930553AE-3ECA-43AF-B854-5E314F27217C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4009C896-86BF-48DF-9D05-7452F3FD9F50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2865" windowWidth="27675" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1125" yWindow="3120" windowWidth="27675" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>Id</t>
   </si>
@@ -78,14 +78,6 @@
       </rPr>
       <t>nIdleEvent</t>
     </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>拾取</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>OnPickUpItemEvent</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -145,15 +137,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -460,10 +449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -541,22 +530,11 @@
       <c r="A7" s="1">
         <v>1009</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A8" s="1">
-        <v>1011</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>